<commit_message>
added sendtoendnote scripts and commited
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>TCID</t>
   </si>
@@ -53,17 +53,26 @@
     <t>ENW001</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>Need to add test case description</t>
+    <t>ENW002</t>
+  </si>
+  <si>
+    <t>OPQA-1678</t>
+  </si>
+  <si>
+    <t>OPQA_1679</t>
+  </si>
+  <si>
+    <t>Verify that user is able to send the record from below following pages: •Summary lists (for Article, Patent, and Post items)</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to send the only one record at a time from article,Post,Patent view Pages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +149,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -186,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,9 +235,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,6 +270,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,14 +446,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -443,7 +462,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,22 +479,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -484,20 +516,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -511,7 +543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>49</v>
       </c>
@@ -525,7 +557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50</v>
       </c>
@@ -539,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
send to endnote linking flows
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="IAM005" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>TCID</t>
   </si>
@@ -29,21 +28,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
-    <t>VALIDITY</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>CHARACTER LENGTH</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
@@ -62,30 +46,56 @@
     <t>OPQA_1679</t>
   </si>
   <si>
-    <t>Verify that user is able to send the record from below following pages: •Summary lists (for Article, Patent, and Post items)</t>
-  </si>
-  <si>
     <t>Verify that the user is able to send the only one record at a time from article,Post,Patent view Pages</t>
+  </si>
+  <si>
+    <t>ENW003</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>ENW004</t>
+  </si>
+  <si>
+    <t>ENW005</t>
+  </si>
+  <si>
+    <t>ENW006</t>
+  </si>
+  <si>
+    <t>Verify that user is able to send the record from below following pages: Verify that user is able to send the record from Summary lists(Search Result page for Article, Patent, and Post items)</t>
+  </si>
+  <si>
+    <t>Verify that the linking modal to link steam account displayed when user clicks on the export button when user is signed in using facebook/linkedIn account and user is having steam account which is not linked to facebook/LinkedIn</t>
+  </si>
+  <si>
+    <t>OPQA-1699</t>
+  </si>
+  <si>
+    <t>Verify that the "Thanks for your interest in EndNote......" modal displayed when user clicks on the export button when user is signed to facebook account and not having existing steam account||Verify that the 'Link accounts' Modal displayed when user clicks on 'Yes, I have account' button to link steam account in ENW with different email id in linking Modal||User who is signed in using social account,After clicking the export to ENW button, user should be able to see the options to either provide STeAM credentials with different emailid or register a new STeAM account||Verify that the steam account is linked to social account, after providing steam credentials with different email address in 'link Acounts' Modal and record will be sent to ENW &amp; steam Email id will be saved as alternative email id</t>
+  </si>
+  <si>
+    <t>OPQA-1701||OPQA-1710||OPQA-1750||OPQA-1757</t>
+  </si>
+  <si>
+    <t>OPQA-1699||OPQA-1770</t>
+  </si>
+  <si>
+    <t>Verify that the linking modal to link steam account displayed when user clicks on the export button when user is signed in using facebook/linkedIn account and user is having steam account which is not linked to facebook/LinkedIn||Verify that the user shall be able to exit the linking process through clicking [x] on the page and clicking outside the Modal results in Linking Modal to disappear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -126,25 +136,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -476,114 +479,94 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>49</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>50</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>51</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed scripts as per chinna's suggestion
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>TCID</t>
   </si>
@@ -52,9 +52,6 @@
     <t>ENW003</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>ENW004</t>
   </si>
   <si>
@@ -83,6 +80,12 @@
   </si>
   <si>
     <t>Verify that the linking modal to link steam account displayed when user clicks on the export button when user is signed in using facebook/linkedIn account and user is having steam account which is not linked to facebook/LinkedIn||Verify that the user shall be able to exit the linking process through clicking [x] on the page and clicking outside the Modal results in Linking Modal to disappear</t>
+  </si>
+  <si>
+    <t>Verify that the "Thanks for your interest in EndNote......" modal displayed when user clicks on the export button when user is signed to facebook account and not having existing steam account</t>
+  </si>
+  <si>
+    <t>OPQA-1701</t>
   </si>
 </sst>
 </file>
@@ -452,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +508,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -517,10 +520,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -529,42 +532,46 @@
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2"/>
     </row>

</xml_diff>

<commit_message>
Feedback forms are commited
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>TCID</t>
   </si>
@@ -86,6 +86,128 @@
   </si>
   <si>
     <t>OPQA-1701</t>
+  </si>
+  <si>
+    <t>ENW009</t>
+  </si>
+  <si>
+    <t>OPQA-3605 
+|| OPQA-3607</t>
+  </si>
+  <si>
+    <t>Verify that Alternate header should be displayed for all users who access a page hosted by the Endnote platform and Non-market test group users  
+|| Verify that Alternate Endnote header should replace Neon logo with "Thomson Reuters" text without the hot link and should not allow user to Navigate to Neon for Non-market test group users</t>
+  </si>
+  <si>
+    <t>ENW010</t>
+  </si>
+  <si>
+    <t>OPQA-3571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Verify that the alternate Endnote profile fly out should look like the ENW alt_App and 
+a. User name NOT hyperlinked to Profile page
+b. No "More" link to Profile page
+c. Display profile image if available
+</t>
+  </si>
+  <si>
+    <t>ENW011</t>
+  </si>
+  <si>
+    <t>OPQA-3577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the alternate Endnote profile fly out should only display the first and last name pulled from STeAM account, when STeAM account does not have a TRUID </t>
+  </si>
+  <si>
+    <t>ENW012</t>
+  </si>
+  <si>
+    <t>OPQA-3582</t>
+  </si>
+  <si>
+    <t>Verify that the alternate Endnote profile fly out should contain "Privacy" link, which should Open new browser window with static page displaying the privacy statement content.</t>
+  </si>
+  <si>
+    <t>ENW013</t>
+  </si>
+  <si>
+    <t>OPQA-3585</t>
+  </si>
+  <si>
+    <t>Verify that the alternate Endnote profile fly out should contain "Terms of use" link ,which should Open a new browser window with static page displaying the terms of use content</t>
+  </si>
+  <si>
+    <t>ENW014</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OPQA-3587</t>
+  </si>
+  <si>
+    <t>Verify that the alternate Endnote profile fly out should contain "help" link, which should take the user to existing Endnote help page which is hosted on Endnote stack.</t>
+  </si>
+  <si>
+    <t>ENW015</t>
+  </si>
+  <si>
+    <t>OPQA-3589</t>
+  </si>
+  <si>
+    <t>Verify that the alternate Endnote profile fly out should contain "Feedback" link, which should take the user to the existing (BAU) version of the Endnote Feedback form.</t>
+  </si>
+  <si>
+    <t>ENW016</t>
+  </si>
+  <si>
+    <t>OPQA-3591</t>
+  </si>
+  <si>
+    <t>Verify that the alternate Endnote profile fly out should provide the ability for a user to log out of Endnote.</t>
+  </si>
+  <si>
+    <t>ENW017</t>
+  </si>
+  <si>
+    <t>ENW018</t>
+  </si>
+  <si>
+    <t>Verify that the Neon specific Feedback page is displayed, When a user is navigating from Neon 
+|| Verify that,the user's message should be sent to a configurable email box specific for Neon when user submitting the feedback from Neon version of the new "Feedback" page.</t>
+  </si>
+  <si>
+    <t>OPQA-2158 
+||OPQA-2161</t>
+  </si>
+  <si>
+    <t>After submitting request on Neon feedback page by clicking "Report a problem or submit a support request" hyperlink. "Your support request has been submitted." Message should be displayed.</t>
+  </si>
+  <si>
+    <t>ENW019</t>
+  </si>
+  <si>
+    <t>OPQA-3171</t>
+  </si>
+  <si>
+    <t>ENW020</t>
+  </si>
+  <si>
+    <t>OPQA-2157 
+||OPQA-2159 
+||OPQA-3171</t>
+  </si>
+  <si>
+    <t>Verify that the  Endnote profile fly out should contain "Feedback" link, which should take the user to the Neon version of the Endnote Feedback form.                || And Verify that,the user's message should be sent to a configurable email box specific for Endnote, when user submitting a message in the help input form on the Endnote version of the new "Feedback" page
+||After submitting request on Endnote version of the Neon feedback page by clicking "Report a problem or submit a support request" hyperlink. "Your support request has been submitted." Message should be displayed.</t>
+  </si>
+  <si>
+    <t>Verify that user who is navigated to the community enabled version of Endnote via WOS navigation in page, upon clicking Account,Profile, feedback and Project Neon link in Profileflyout user will be taken to ENW login page and after entering credentials it should take  to correct destination pages.</t>
+  </si>
+  <si>
+    <t>OPQA-3629</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -142,12 +264,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -209,7 +338,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,7 +373,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -453,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,6 +704,186 @@
       </c>
       <c r="E7" s="2"/>
     </row>
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Developed Scripts in ENW Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
   <si>
     <t>TCID</t>
   </si>
@@ -209,12 +209,30 @@
   <si>
     <t>N</t>
   </si>
+  <si>
+    <t>ENW000010</t>
+  </si>
+  <si>
+    <t>ENW000012</t>
+  </si>
+  <si>
+    <t>ENW000011</t>
+  </si>
+  <si>
+    <t>steam Login  account page</t>
+  </si>
+  <si>
+    <t>ENW00029</t>
+  </si>
+  <si>
+    <t>Social Login account page</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -260,11 +278,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -277,6 +306,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -370,7 +403,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -405,7 +437,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -581,14 +612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A20" sqref="A20:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -597,7 +628,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -629,7 +660,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -644,7 +675,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="90">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -659,7 +690,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="60">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -674,7 +705,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="165">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -689,7 +720,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -704,7 +735,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -719,7 +750,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="90">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -734,7 +765,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -749,7 +780,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -764,7 +795,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="45">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
@@ -779,7 +810,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="45">
       <c r="A13" s="4" t="s">
         <v>39</v>
       </c>
@@ -794,7 +825,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="45">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -809,7 +840,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
@@ -824,7 +855,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="120">
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
@@ -839,7 +870,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="75">
       <c r="A17" s="4" t="s">
         <v>49</v>
       </c>
@@ -854,7 +885,7 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
@@ -869,7 +900,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="4" t="s">
         <v>55</v>
       </c>
@@ -883,6 +914,62 @@
         <v>60</v>
       </c>
       <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="45">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modified scripts in ENW module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>TCID</t>
   </si>
@@ -219,13 +219,28 @@
     <t>ENW000011</t>
   </si>
   <si>
-    <t>steam Login  account page</t>
-  </si>
-  <si>
     <t>ENW00029</t>
   </si>
   <si>
-    <t>Social Login account page</t>
+    <t xml:space="preserve"> OPQA-1968||OPQA-1969 ||OPQA-1970||OPQA-1979||OPQA-1986||OPQA-3864 </t>
+  </si>
+  <si>
+    <t>Fb login with account setting page linking modal</t>
+  </si>
+  <si>
+    <t>LI login with account setting page linking modal</t>
+  </si>
+  <si>
+    <t>OPQA-1919||OPQA-1915</t>
+  </si>
+  <si>
+    <t>steam login</t>
+  </si>
+  <si>
+    <t>OPQA-3196</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to see all emails that are associated to my Neon identity under the account page</t>
   </si>
 </sst>
 </file>
@@ -255,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -278,22 +293,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -306,10 +310,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,14 +615,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="70.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -915,59 +915,59 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="45">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" ht="75">
+      <c r="A20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45">
-      <c r="A21" t="s">
+      <c r="B20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60">
+      <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="B21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="7" t="s">
+      <c r="B23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed ENW Scripts- srini
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -638,7 +638,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed all xls test cases with || symbol, Added Jira id navigation code in Testbase.java
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -40,9 +40,6 @@
     <t>OPQA-1678</t>
   </si>
   <si>
-    <t>OPQA_1679</t>
-  </si>
-  <si>
     <t>Verify that the user is able to send the only one record at a time from article,Post,Patent view Pages</t>
   </si>
   <si>
@@ -262,12 +259,15 @@
   <si>
     <t>ENW022</t>
   </si>
+  <si>
+    <t>OPQA-1679</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,7 +423,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -458,7 +457,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -634,14 +632,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="25.5703125" customWidth="1" collapsed="1"/>
@@ -650,7 +648,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,25 +662,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -690,352 +688,352 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="75">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="45">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="135">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="45">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="75">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="75">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="30">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="120">
+      <c r="A17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="45">
+      <c r="A18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="60">
+      <c r="A19" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="45">
+      <c r="A20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="60">
+      <c r="A21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="60">
+      <c r="A22" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="60">
+      <c r="A23" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="60">
+      <c r="A24" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="75">
+      <c r="A25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
commiting the Watchlist and ENW script fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -227,10 +227,6 @@
     <t>ENW007</t>
   </si>
   <si>
-    <t xml:space="preserve">OPQA-2157 
-||OPQA-2159 </t>
-  </si>
-  <si>
     <t>After submitting request on Endnote version of the Neon feedback page by clicking "Report a problem or submit a support request" hyperlink. "Your support request has been submitted." Message should be displayed.</t>
   </si>
   <si>
@@ -256,9 +252,6 @@
   </si>
   <si>
     <t>Verify that the Reference type","Title","Journal,Volume,Issue,Pagenumber,Times cited,Cited Refrence count,URL in ENDnote from Neon for Article</t>
-  </si>
-  <si>
-    <t>Verify that the  Endnote profile fly out should contain "Feedback" link, which should take the user to the Neon version of the Endnote Feedback form.                || And Verify that,the user's message should be sent to a configurable email box specific for Endnote, when user submitting a message in the help input form on the Endnote version of the new "Feedback" page</t>
   </si>
   <si>
     <t>OPQA-2329 
@@ -272,6 +265,16 @@
     <t>Clicking[x] on Neon side Linking Modals
 Clicking 'not now' from Neon side Linking Modals
 Clicking outside the Modal from Neon side Linking Modals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPQA-3575
+||OPQA-2157 
+||OPQA-2159 </t>
+  </si>
+  <si>
+    <t>Verify that user shall be sent to Community enabled version of Endnote while user sign in to the ENW through STeAM or Social as a first time,when the user is affiliated to a Customer in the market test group based on the WOS Customer Check.
+||Verify that the  Endnote profile fly out should contain "Feedback" link, which should take the user to the Neon version of the Endnote Feedback form.               
+ || And Verify that,the user's message should be sent to a configurable email box specific for Endnote, when user submitting a message in the help input form on the Endnote version of the new "Feedback" page</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -773,10 +776,10 @@
         <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -788,7 +791,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>23</v>
@@ -903,15 +906,15 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -920,13 +923,13 @@
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
@@ -935,13 +938,13 @@
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -995,13 +998,13 @@
     </row>
     <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added OPQA-3334 to enw006
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -76,12 +76,6 @@
     <t>Verify that the linking modal to link steam account displayed when user clicks on the export button when user is signed in using facebook/linkedIn account and user is having steam account which is not linked to facebook/LinkedIn||Verify that the user shall be able to exit the linking process through clicking [x] on the page and clicking outside the Modal results in Linking Modal to disappear</t>
   </si>
   <si>
-    <t>Verify that the "Thanks for your interest in EndNote......" modal displayed when user clicks on the export button when user is signed to facebook account and not having existing steam account</t>
-  </si>
-  <si>
-    <t>OPQA-1701</t>
-  </si>
-  <si>
     <t>ENW009</t>
   </si>
   <si>
@@ -293,6 +287,12 @@
   </si>
   <si>
     <t>Verify that the Reference type","Title",URL in ENDnote from Neon for Posts</t>
+  </si>
+  <si>
+    <t>OPQA-1701||OPQA-3290</t>
+  </si>
+  <si>
+    <t>Verify that the "Thanks for your interest in EndNote......" modal displayed when user clicks on the export button when user is signed to facebook account and not having existing steam account||Verify that,after clicking "send to Endnote" Button,user should be able to see the text "Enter you existing account credential (CortellisTM, EndNoteTM Online,InCitesTM, ResearcherID,Thomson InnovationTM, Web of ScienceTM) to link your accounts."</t>
   </si>
 </sst>
 </file>
@@ -670,7 +670,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -704,7 +704,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -774,15 +774,15 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3</v>
@@ -791,13 +791,13 @@
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -806,13 +806,13 @@
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -821,13 +821,13 @@
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
@@ -836,13 +836,13 @@
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -851,13 +851,13 @@
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>3</v>
@@ -866,13 +866,13 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -881,13 +881,13 @@
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -896,13 +896,13 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>3</v>
@@ -911,13 +911,13 @@
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>3</v>
@@ -926,13 +926,13 @@
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -941,13 +941,13 @@
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
@@ -956,13 +956,13 @@
     </row>
     <row r="19" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -971,13 +971,13 @@
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>3</v>
@@ -1001,13 +1001,13 @@
     </row>
     <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>3</v>
@@ -1016,13 +1016,13 @@
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>3</v>
@@ -1031,13 +1031,13 @@
     </row>
     <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>3</v>
@@ -1046,13 +1046,13 @@
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>3</v>
@@ -1061,13 +1061,13 @@
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>3</v>
@@ -1076,13 +1076,13 @@
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1091,13 +1091,13 @@
     </row>
     <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1106,13 +1106,13 @@
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated Enw and ENWIAM.xls files
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="13290" windowHeight="3780"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
   <si>
     <t>TCID</t>
   </si>
@@ -303,6 +303,34 @@
     <t>Verify that user who is navigated to the community enabled version of Endnote via WOS navigation in page, upon clicking Account,Profile, feedback and Project Neon link in Profileflyout user will be taken to ENW login page and after entering credentials it should take  to correct destination pages.
 || Verify that, Users who navigate from WOS to ENW with a valid WOS session, should be taken to ENW in a signed in state
 Verify that,user can navigate from WOS to ENW,if the user is affiliated to a Customer in the market test group based on the WOS Customer Check, and should be sent to the Community enabled version of Endnote.</t>
+  </si>
+  <si>
+    <t>ENW024</t>
+  </si>
+  <si>
+    <t>Verify that,user can navigate from WOS to ENW,if the user is not affiliated to a Customer in the market test group based on the WOS Customer Check, and should be sent to the alternate version of Endnote.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+OPQA-3590</t>
+  </si>
+  <si>
+    <t>Verify that non personalized user who navigates from WOS to ENW by clicking the ENW icon from search results shall be sent to the ENW sign in screen for authentication</t>
+  </si>
+  <si>
+    <t>QAOPQA-2733</t>
+  </si>
+  <si>
+    <t>ENW025</t>
+  </si>
+  <si>
+    <t>OPQA-2730</t>
+  </si>
+  <si>
+    <t>Verify that personalized user who navigates from WOS to ENW by clicking the ENW icon from search results shall be automatically signed into ENW and taken to the full record</t>
+  </si>
+  <si>
+    <t>ENW026</t>
   </si>
 </sst>
 </file>
@@ -677,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,64 +1098,109 @@
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="A26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="D28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added opqa-2288 to enw003
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2700" windowWidth="13290" windowHeight="3780"/>
@@ -67,12 +67,6 @@
     <t>OPQA-1701||OPQA-1710||OPQA-1750||OPQA-1757</t>
   </si>
   <si>
-    <t>OPQA-1699||OPQA-1770</t>
-  </si>
-  <si>
-    <t>Verify that the linking modal to link steam account displayed when user clicks on the export button when user is signed in using facebook/linkedIn account and user is having steam account which is not linked to facebook/LinkedIn||Verify that the user shall be able to exit the linking process through clicking [x] on the page and clicking outside the Modal results in Linking Modal to disappear</t>
-  </si>
-  <si>
     <t>ENW009</t>
   </si>
   <si>
@@ -331,6 +325,12 @@
   </si>
   <si>
     <t>ENW026</t>
+  </si>
+  <si>
+    <t>Verify that the linking modal to link steam account displayed when user clicks on the export button when user is signed in using facebook/linkedIn account and user is having steam account which is not linked to facebook/LinkedIn||Verify that the user shall be able to exit the linking process through clicking [x] on the page and clicking outside the Modal results in Linking Modal to disappear||Verify that when linking a STeAM with a matching email, the user should receive error message '" The email and password do not match. Please try again." if he gives incorrect password.</t>
+  </si>
+  <si>
+    <t>OPQA-1699||OPQA-1770||OPQA-2288</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,7 +496,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -708,7 +708,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +734,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -742,10 +742,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -767,15 +767,15 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -817,10 +817,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3</v>
@@ -829,13 +829,13 @@
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -844,13 +844,13 @@
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -859,13 +859,13 @@
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
@@ -874,13 +874,13 @@
     </row>
     <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -889,13 +889,13 @@
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>3</v>
@@ -904,13 +904,13 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -919,13 +919,13 @@
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -934,13 +934,13 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>3</v>
@@ -949,13 +949,13 @@
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>3</v>
@@ -964,13 +964,13 @@
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>3</v>
@@ -979,13 +979,13 @@
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
@@ -994,13 +994,13 @@
     </row>
     <row r="19" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1009,13 +1009,13 @@
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1024,13 +1024,13 @@
     </row>
     <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>3</v>
@@ -1039,13 +1039,13 @@
     </row>
     <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>3</v>
@@ -1054,13 +1054,13 @@
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>3</v>
@@ -1069,13 +1069,13 @@
     </row>
     <row r="24" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>3</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>3</v>
@@ -1099,13 +1099,13 @@
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>3</v>
@@ -1114,13 +1114,13 @@
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1129,13 +1129,13 @@
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1144,13 +1144,13 @@
     </row>
     <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1159,13 +1159,13 @@
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>3</v>
@@ -1174,13 +1174,13 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>3</v>
@@ -1189,13 +1189,13 @@
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
added jiraids to ENW,ENWIAM,IAM xls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2760" windowWidth="13290" windowHeight="3720"/>
@@ -251,12 +251,6 @@
     <t>Verify that the "Thanks for your interest in EndNote......" modal displayed when user clicks on the export button when user is signed to facebook account and not having existing steam account||Verify that,after clicking "send to Endnote" Button,user should be able to see the text "Enter you existing account credential (CortellisTM, EndNoteTM Online,InCitesTM, ResearcherID,Thomson InnovationTM, Web of ScienceTM) to link your accounts."</t>
   </si>
   <si>
-    <t>OPQA-1679||OPQA-3642</t>
-  </si>
-  <si>
-    <t>Verify that the user is able to send the only one record at a time from article,Post,Patent view Pages||Verify that Non Market test group user who signed into the community application should be able to send a record to endnote.</t>
-  </si>
-  <si>
     <t>OPQA-1701||OPQA-3334</t>
   </si>
   <si>
@@ -369,6 +363,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Verify that Non Market test group user who signed into the community application should be able to navigate to the alternate version of Endnote through "EndNote Online" link on App switcher, When STeAM account is linked</t>
+  </si>
+  <si>
+    <t>OPQA-1679||OPQA-3642||OPQA-1791</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to send the only one record at a time from article,Post,Patent view Pages||Verify that Non Market test group user who signed into the community application should be able to send a record to endnote.||Verify that User is able to sign-into EndNote Web with valid credentials</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -534,7 +534,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,15 +775,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -810,10 +810,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -855,7 +855,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>74</v>
@@ -915,10 +915,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -960,10 +960,10 @@
         <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1065,10 +1065,10 @@
         <v>65</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>3</v>
@@ -1110,10 +1110,10 @@
         <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>3</v>
@@ -1137,13 +1137,13 @@
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>3</v>
@@ -1212,13 +1212,13 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>3</v>
@@ -1227,13 +1227,13 @@
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>3</v>
@@ -1242,13 +1242,13 @@
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>3</v>
@@ -1257,13 +1257,13 @@
     </row>
     <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>3</v>
@@ -1272,13 +1272,13 @@
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>3</v>
@@ -1287,13 +1287,13 @@
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
enw033 added for opqa-1942
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="112">
   <si>
     <t>TCID</t>
   </si>
@@ -369,6 +369,15 @@
   </si>
   <si>
     <t>Verify that the user is able to send the only one record at a time from article,Post,Patent view Pages||Verify that Non Market test group user who signed into the community application should be able to send a record to endnote.||Verify that User is able to sign-into EndNote Web with valid credentials</t>
+  </si>
+  <si>
+    <t>ENW033</t>
+  </si>
+  <si>
+    <t>OPQA-1942||OPQA-3731</t>
+  </si>
+  <si>
+    <t>Verify that a Neon account can only have 1 Facebook, 1 LinkedIn, and 1 STeAM account linked.||Verify that,On ENW user should get "Unable to link" message, while attempt linking with STeAM and sign into social account,whose STeAM account is already linked with different social account.</t>
   </si>
 </sst>
 </file>
@@ -743,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C40" sqref="C38:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,33 +1281,48 @@
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" s="4"/>
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added enw035 for opqa-1713,
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -378,6 +378,15 @@
   </si>
   <si>
     <t>Verify that a Neon account can only have 1 Facebook, 1 LinkedIn, and 1 STeAM account linked.||Verify that,On ENW user should get "Unable to link" message, while attempt linking with STeAM and sign into social account,whose STeAM account is already linked with different social account.</t>
+  </si>
+  <si>
+    <t>ENW035</t>
+  </si>
+  <si>
+    <t>OPQA-1713</t>
+  </si>
+  <si>
+    <t>Verify that the error should be displayed when there is not enough space in enw to accept the Neon records after clicking send to ENDNote button</t>
   </si>
 </sst>
 </file>
@@ -752,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C40" sqref="C38:C40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,6 +1333,21 @@
       </c>
       <c r="E37" s="4"/>
     </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ENW Fixes has been committed
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2760" windowWidth="13290" windowHeight="3720"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="118">
   <si>
     <t>TCID</t>
   </si>
@@ -387,6 +387,18 @@
   </si>
   <si>
     <t>Verify that the error should be displayed when there is not enough space in enw to accept the Neon records after clicking send to ENDNote button</t>
+  </si>
+  <si>
+    <t>ENW019A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+OPQA-3643</t>
+  </si>
+  <si>
+    <t>Verify that the Neon specific Feedback page is displayed, When a user is navigating from Neon . "For Non Market user "        
+ ||After submitting request on Endnote version of the Neon feedback page by clicking "Report a problem or submit a support request" hyperlink. "Your support request has been submitted." Message should be displayed.
+|| Verify that Non Market test group user who signed into the community application should be able to navigate to the alternate version of Endnote through "EndNote Online" link on App switcher, When STeAM account is linked.</t>
   </si>
 </sst>
 </file>
@@ -517,7 +529,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -552,7 +564,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -761,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,210 +1075,210 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="D21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="D22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="D24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="D26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="D30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>3</v>
@@ -1275,28 +1287,28 @@
     </row>
     <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>3</v>
@@ -1305,48 +1317,63 @@
     </row>
     <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" s="4"/>
+      <c r="D39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added enw036 for opqa-3295
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2760" windowWidth="13290" windowHeight="3720"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="121">
   <si>
     <t>TCID</t>
   </si>
@@ -211,9 +211,6 @@
     <t>ENW022</t>
   </si>
   <si>
-    <t>OPQA-3290||OPQA-3297||OPQA-3299||OPQA-3301||OPQA-3312||OPQA-3313||OPQA-3317||OPQA-3318||OPQA-3319</t>
-  </si>
-  <si>
     <t>Verify that the Reference type","Title","Journal,Volume,Issue,Pagenumber,Times cited,Cited Refrence count,URL in ENDnote from Neon for Article</t>
   </si>
   <si>
@@ -399,6 +396,18 @@
     <t>Verify that the Neon specific Feedback page is displayed, When a user is navigating from Neon . "For Non Market user "        
  ||After submitting request on Endnote version of the Neon feedback page by clicking "Report a problem or submit a support request" hyperlink. "Your support request has been submitted." Message should be displayed.
 || Verify that Non Market test group user who signed into the community application should be able to navigate to the alternate version of Endnote through "EndNote Online" link on App switcher, When STeAM account is linked.</t>
+  </si>
+  <si>
+    <t>OPQA-3290||OPQA-3297||OPQA-3299||OPQA-3301||OPQA-3312||OPQA-3313||OPQA-3317||OPQA-3318||OPQA-3319||OPQA-1793</t>
+  </si>
+  <si>
+    <t>ENW036</t>
+  </si>
+  <si>
+    <t>Verify that field "Group Authors" in Neon should be displayed as "Author" label in Endnote after exporting the article from Neon to ENW.</t>
+  </si>
+  <si>
+    <t>OPQA-3295</t>
   </si>
 </sst>
 </file>
@@ -529,7 +538,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -564,7 +573,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -773,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,10 +819,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -840,10 +849,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -885,25 +894,25 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -912,13 +921,13 @@
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -927,13 +936,13 @@
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
@@ -945,10 +954,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -990,10 +999,10 @@
         <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>3</v>
@@ -1065,10 +1074,10 @@
         <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1077,13 +1086,13 @@
     </row>
     <row r="20" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1107,13 +1116,13 @@
     </row>
     <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>3</v>
@@ -1155,10 +1164,10 @@
         <v>44</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>3</v>
@@ -1182,13 +1191,13 @@
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>3</v>
@@ -1257,13 +1266,13 @@
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>3</v>
@@ -1272,13 +1281,13 @@
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>3</v>
@@ -1287,13 +1296,13 @@
     </row>
     <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>3</v>
@@ -1302,13 +1311,13 @@
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>3</v>
@@ -1317,13 +1326,13 @@
     </row>
     <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>3</v>
@@ -1332,13 +1341,13 @@
     </row>
     <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>3</v>
@@ -1347,13 +1356,13 @@
     </row>
     <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>3</v>
@@ -1362,18 +1371,33 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="D39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commits the ENW changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="131">
   <si>
     <t>TCID</t>
   </si>
@@ -431,6 +431,17 @@
   <si>
     <t>Verify that the user is able to login to EndNote Web support utility with using valid credentials
 || Verify that If the WoS Customer Association check determines that the user is part of the WoS market test group, then the user will get access to the  "Community enabled version of ENW"</t>
+  </si>
+  <si>
+    <t>ENW042</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OPQA-3598
+||OPQA-3599</t>
+  </si>
+  <si>
+    <t>Verify that the user signed in to community enabled version of Endnote and having valid Neon session will be taken to Profile page seamlessly by clicking on the profilename in profile flyout
+|| Verify that the user signed in to community enabled version of Endnote and having valid Neon session will be taken to Account page seamlessly by clicking on the Account in profile flyout</t>
   </si>
 </sst>
 </file>
@@ -805,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,6 +1463,21 @@
       </c>
       <c r="E42" s="4"/>
     </row>
+    <row r="43" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New ENW developed scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
   <si>
     <t>TCID</t>
   </si>
@@ -442,6 +442,16 @@
   <si>
     <t>Verify that the user signed in to community enabled version of Endnote and having valid Neon session will be taken to Profile page seamlessly by clicking on the profilename in profile flyout
 || Verify that the user signed in to community enabled version of Endnote and having valid Neon session will be taken to Account page seamlessly by clicking on the Account in profile flyout</t>
+  </si>
+  <si>
+    <t>ENW043</t>
+  </si>
+  <si>
+    <t>Verify that the user signed in to community enabled version of Endnote and having invalid Neon session will be taken to Privacy page seamlessly by clicking on the Privacy in profile flyout.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+OPQA-3617</t>
   </si>
 </sst>
 </file>
@@ -816,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,6 +1488,21 @@
       </c>
       <c r="E43" s="4"/>
     </row>
+    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
IPA and ENW login page and Xls fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="137">
   <si>
     <t>TCID</t>
   </si>
@@ -452,6 +452,18 @@
   <si>
     <t xml:space="preserve">
 OPQA-3617</t>
+  </si>
+  <si>
+    <t>ENW044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+OPQA-3683
+||OPQA-3684</t>
+  </si>
+  <si>
+    <t>Verify that field "Patent IPC Codes" in Neon should be displayed as "Keywords" label in Endnote after exporting the patent from Neon to ENW.
+||Verify that field "Patent Assignee" in Neon should be displayed as "Assignee" label in Endnote after exporting the patent from Neon to ENW.</t>
   </si>
 </sst>
 </file>
@@ -826,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,6 +1515,21 @@
       </c>
       <c r="E44" s="4"/>
     </row>
+    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ENW Fixes have been committed
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -435,15 +435,6 @@
     <t>ENW044</t>
   </si>
   <si>
-    <t xml:space="preserve">
-OPQA-3683
-||OPQA-3684</t>
-  </si>
-  <si>
-    <t>Verify that field "Patent IPC Codes" in Neon should be displayed as "Keywords" label in Endnote after exporting the patent from Neon to ENW.
-||Verify that field "Patent Assignee" in Neon should be displayed as "Assignee" label in Endnote after exporting the patent from Neon to ENW.</t>
-  </si>
-  <si>
     <t>OPQA-3605 || OPQA-3607 
 || OPQA-3576 ||OPQA-3571</t>
   </si>
@@ -457,12 +448,19 @@
 c. Display profile image if available
 </t>
   </si>
+  <si>
+    <t xml:space="preserve">
+OPQA-3694</t>
+  </si>
+  <si>
+    <t>Verify that the the body of the Post should be displyed under the Abstract field On Reference page Optional Fields in EndNote, after post record exported</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,8 +468,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +486,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -524,6 +535,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -832,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,10 +1016,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1492,15 +1506,15 @@
       </c>
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
added OPQA-3196 to enwiam052
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2760" windowWidth="13290" windowHeight="3720"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="131">
   <si>
     <t>TCID</t>
   </si>
@@ -150,9 +150,6 @@
     <t>ENW000012</t>
   </si>
   <si>
-    <t>ENW000011</t>
-  </si>
-  <si>
     <t>ENW00029</t>
   </si>
   <si>
@@ -166,12 +163,6 @@
   </si>
   <si>
     <t>OPQA-1919||OPQA-1915</t>
-  </si>
-  <si>
-    <t>OPQA-3196</t>
-  </si>
-  <si>
-    <t>As a user, I want to be able to see all emails that are associated to my Neon identity under the account page</t>
   </si>
   <si>
     <t>Results</t>
@@ -600,7 +591,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,7 +626,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -844,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +864,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -881,10 +872,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -911,10 +902,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -956,10 +947,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3</v>
@@ -968,13 +959,13 @@
     </row>
     <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -983,13 +974,13 @@
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -998,13 +989,13 @@
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
@@ -1016,10 +1007,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1046,10 +1037,10 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -1121,10 +1112,10 @@
         <v>34</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
@@ -1133,13 +1124,13 @@
     </row>
     <row r="19" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1148,13 +1139,13 @@
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1163,13 +1154,13 @@
     </row>
     <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>3</v>
@@ -1211,10 +1202,10 @@
         <v>41</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>3</v>
@@ -1223,13 +1214,13 @@
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>3</v>
@@ -1238,13 +1229,13 @@
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>3</v>
@@ -1256,10 +1247,10 @@
         <v>42</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1271,10 +1262,10 @@
         <v>43</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1283,13 +1274,13 @@
     </row>
     <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1297,16 +1288,16 @@
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>44</v>
+      <c r="A30" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="4"/>
@@ -1316,25 +1307,25 @@
         <v>82</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="D31" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>3</v>
@@ -1343,28 +1334,28 @@
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="D33" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>3</v>
@@ -1373,20 +1364,20 @@
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>103</v>
+        <v>91</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>94</v>
       </c>
@@ -1401,15 +1392,15 @@
       </c>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>3</v>
@@ -1418,13 +1409,13 @@
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>3</v>
@@ -1433,21 +1424,21 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -1461,7 +1452,7 @@
       </c>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>120</v>
       </c>
@@ -1476,50 +1467,35 @@
       </c>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="D42" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ENW updated scripts have been committed
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2760" windowWidth="13290" windowHeight="3720"/>
@@ -359,11 +359,6 @@
 OPQA-3643</t>
   </si>
   <si>
-    <t>Verify that the Neon specific Feedback page is displayed, When a user is navigating from Neon . "For Non Market user "        
- ||After submitting request on Endnote version of the Neon feedback page by clicking "Report a problem or submit a support request" hyperlink. "Your support request has been submitted." Message should be displayed.
-|| Verify that Non Market test group user who signed into the community application should be able to navigate to the alternate version of Endnote through "EndNote Online" link on App switcher, When STeAM account is linked.</t>
-  </si>
-  <si>
     <t>OPQA-3290||OPQA-3297||OPQA-3299||OPQA-3301||OPQA-3312||OPQA-3313||OPQA-3317||OPQA-3318||OPQA-3319||OPQA-1793</t>
   </si>
   <si>
@@ -445,6 +440,9 @@
   </si>
   <si>
     <t>Verify that the the body of the Post should be displyed under the Abstract field On Reference page Optional Fields in EndNote, after post record exported</t>
+  </si>
+  <si>
+    <t>Verify that Non Market test group user who signed into the community application should be able to navigate to the alternate version of Endnote through "EndNote Online" link on App switcher, When STeAM account is linked.</t>
   </si>
 </sst>
 </file>
@@ -591,7 +589,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -626,7 +624,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -837,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,7 +960,7 @@
         <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>56</v>
@@ -1007,10 +1005,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1122,7 +1120,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>105</v>
       </c>
@@ -1130,7 +1128,7 @@
         <v>106</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1142,10 +1140,10 @@
         <v>55</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1409,13 +1407,13 @@
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>3</v>
@@ -1424,13 +1422,13 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>3</v>
@@ -1439,13 +1437,13 @@
     </row>
     <row r="40" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>3</v>
@@ -1454,13 +1452,13 @@
     </row>
     <row r="41" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>3</v>
@@ -1469,13 +1467,13 @@
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>3</v>
@@ -1484,13 +1482,13 @@
     </row>
     <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
ENW scripts(ENW037 to ENW044) have been modified and updated
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2760" windowWidth="13290" windowHeight="3720"/>
@@ -128,10 +128,6 @@
 || Verify that,the user's message should be sent to a configurable email box specific for Neon when user submitting the feedback from Neon version of the new "Feedback" page.</t>
   </si>
   <si>
-    <t>OPQA-2158 
-||OPQA-2161</t>
-  </si>
-  <si>
     <t>After submitting request on Neon feedback page by clicking "Report a problem or submit a support request" hyperlink. "Your support request has been submitted." Message should be displayed.</t>
   </si>
   <si>
@@ -353,10 +349,6 @@
   </si>
   <si>
     <t>ENW019A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-OPQA-3643</t>
   </si>
   <si>
     <t>OPQA-3290||OPQA-3297||OPQA-3299||OPQA-3301||OPQA-3312||OPQA-3313||OPQA-3317||OPQA-3318||OPQA-3319||OPQA-1793</t>
@@ -442,7 +434,15 @@
     <t>Verify that the the body of the Post should be displyed under the Abstract field On Reference page Optional Fields in EndNote, after post record exported</t>
   </si>
   <si>
-    <t>Verify that Non Market test group user who signed into the community application should be able to navigate to the alternate version of Endnote through "EndNote Online" link on App switcher, When STeAM account is linked.</t>
+    <t>Verify that,the user's message should be sent to a configurable email box specific for Neon when user submitting the feedback from Neon version of the new "Feedback" page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+OPQA-2161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPQA-2158 
+</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -870,10 +870,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -900,10 +900,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -945,10 +945,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3</v>
@@ -957,13 +957,13 @@
     </row>
     <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -987,13 +987,13 @@
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>3</v>
@@ -1005,10 +1005,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>3</v>
@@ -1035,10 +1035,10 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -1110,25 +1110,25 @@
         <v>34</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="D18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1137,13 +1137,13 @@
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
@@ -1152,25 +1152,25 @@
     </row>
     <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>36</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>3</v>
@@ -1197,13 +1197,13 @@
     </row>
     <row r="24" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>3</v>
@@ -1212,13 +1212,13 @@
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>3</v>
@@ -1227,13 +1227,13 @@
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>3</v>
@@ -1242,13 +1242,13 @@
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>3</v>
@@ -1257,13 +1257,13 @@
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>3</v>
@@ -1272,13 +1272,13 @@
     </row>
     <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>3</v>
@@ -1287,13 +1287,13 @@
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>3</v>
@@ -1302,13 +1302,13 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>3</v>
@@ -1317,13 +1317,13 @@
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>3</v>
@@ -1332,13 +1332,13 @@
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>3</v>
@@ -1347,13 +1347,13 @@
     </row>
     <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>3</v>
@@ -1362,13 +1362,13 @@
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>3</v>
@@ -1377,13 +1377,13 @@
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>3</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>3</v>
@@ -1407,13 +1407,13 @@
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="C38" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>3</v>
@@ -1422,13 +1422,13 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>3</v>
@@ -1437,13 +1437,13 @@
     </row>
     <row r="40" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>3</v>
@@ -1452,13 +1452,13 @@
     </row>
     <row r="41" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>3</v>
@@ -1467,13 +1467,13 @@
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="C42" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>3</v>
@@ -1482,13 +1482,13 @@
     </row>
     <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added DRA and ENW test cases for sanity job.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/ENW.xlsx
+++ b/src/test/resources/xls/ENW.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="128">
   <si>
     <t>TCID</t>
   </si>
@@ -428,11 +428,20 @@
 1."Project Neon supports linking your accounts - accounts you have for other Thomson Reuters products and social media accounts - so that you can sign in with any of the accounts you already use." should be displayed in account setting page if account is not linked.
 2."Project Neon has linked your accounts. You can sign in with any of the accounts you already use." is displayed when accouts are linked</t>
   </si>
+  <si>
+    <t>ENW045</t>
+  </si>
+  <si>
+    <t>OPQA-2015||OPQA-3650</t>
+  </si>
+  <si>
+    <t>Verify that User is able to sign-into EndNote Web using STeAM.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -817,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,6 +1458,21 @@
       </c>
       <c r="E41" s="4"/>
     </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>